<commit_message>
Enhanced caosce processing to include PAPER III for midwifery
</commit_message>
<xml_diff>
--- a/EXAMS_INTERNAL/ND/ND-2025/RAW_RESULTS/FIRST-YEAR-SECOND-SEMESTER.xlsx
+++ b/EXAMS_INTERNAL/ND/ND-2025/RAW_RESULTS/FIRST-YEAR-SECOND-SEMESTER.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="415">
   <si>
     <t>S/N</t>
   </si>
@@ -1631,7 +1631,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1641,8 +1641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K124"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView topLeftCell="E31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2143,8 +2143,8 @@
       <c r="I14">
         <v>19</v>
       </c>
-      <c r="J14" t="s">
-        <v>389</v>
+      <c r="J14">
+        <v>0</v>
       </c>
       <c r="K14">
         <v>18</v>
@@ -2458,8 +2458,8 @@
       <c r="I23">
         <v>19</v>
       </c>
-      <c r="J23" t="s">
-        <v>389</v>
+      <c r="J23">
+        <v>0</v>
       </c>
       <c r="K23">
         <v>20</v>
@@ -2948,8 +2948,8 @@
       <c r="I37">
         <v>19</v>
       </c>
-      <c r="J37" t="s">
-        <v>389</v>
+      <c r="J37">
+        <v>0</v>
       </c>
       <c r="K37">
         <v>16</v>
@@ -3123,8 +3123,8 @@
       <c r="I42">
         <v>19</v>
       </c>
-      <c r="J42" t="s">
-        <v>389</v>
+      <c r="J42">
+        <v>0</v>
       </c>
       <c r="K42">
         <v>12</v>
@@ -3228,8 +3228,8 @@
       <c r="I45" t="s">
         <v>389</v>
       </c>
-      <c r="J45" t="s">
-        <v>389</v>
+      <c r="J45">
+        <v>0</v>
       </c>
       <c r="K45">
         <v>14</v>
@@ -3257,8 +3257,8 @@
       <c r="G46" s="3">
         <v>18</v>
       </c>
-      <c r="H46" s="4" t="s">
-        <v>389</v>
+      <c r="H46" s="4">
+        <v>0</v>
       </c>
       <c r="I46">
         <v>19</v>
@@ -3292,8 +3292,8 @@
       <c r="G47" s="3">
         <v>15</v>
       </c>
-      <c r="H47" s="4" t="s">
-        <v>389</v>
+      <c r="H47" s="4">
+        <v>0</v>
       </c>
       <c r="I47">
         <v>19</v>
@@ -3327,8 +3327,8 @@
       <c r="G48" s="3">
         <v>15</v>
       </c>
-      <c r="H48" s="4" t="s">
-        <v>389</v>
+      <c r="H48" s="4">
+        <v>0</v>
       </c>
       <c r="I48">
         <v>19</v>
@@ -3998,8 +3998,8 @@
       <c r="I67">
         <v>19</v>
       </c>
-      <c r="J67" t="s">
-        <v>389</v>
+      <c r="J67">
+        <v>0</v>
       </c>
       <c r="K67">
         <v>18</v>
@@ -6010,8 +6010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K124"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="97" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView topLeftCell="A32" zoomScale="97" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10378,8 +10378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="B34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>